<commit_message>
fixed Indri issue in regression
</commit_message>
<xml_diff>
--- a/data/PE2_data.xlsx
+++ b/data/PE2_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfernandezbellon\Dropbox\work\documentaries\sir david\write up\final\supplementary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Kane\Documents\Manuscripts\Documentary paper\documentary-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BC8473-9591-4356-967E-8A786FC2B8E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="411">
   <si>
     <t>African_buffalo</t>
   </si>
@@ -1258,7 +1259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2108,26 +2109,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="123.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="123.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>406</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>403</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>283</v>
@@ -2158,7 +2159,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>284</v>
@@ -2167,7 +2168,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>399</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>194</v>
@@ -2187,7 +2188,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>280</v>
@@ -2196,7 +2197,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>281</v>
@@ -2205,7 +2206,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>285</v>
@@ -2214,7 +2215,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>187</v>
@@ -2223,7 +2224,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>393</v>
       </c>
@@ -2234,7 +2235,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>380</v>
@@ -2243,7 +2244,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>390</v>
       </c>
@@ -2254,7 +2255,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>379</v>
@@ -2263,7 +2264,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>383</v>
@@ -2272,7 +2273,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>384</v>
@@ -2281,7 +2282,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>382</v>
@@ -2297,32 +2298,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H75" sqref="H75"/>
+      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="34.5546875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="31.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -2372,7 +2373,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>196</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -2514,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>200</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -2636,8 +2637,8 @@
       <c r="J7" t="s">
         <v>381</v>
       </c>
-      <c r="K7">
-        <v>44</v>
+      <c r="K7" t="s">
+        <v>198</v>
       </c>
       <c r="L7" t="s">
         <v>46</v>
@@ -2655,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -2669,7 +2670,7 @@
         <v>46</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>218</v>
@@ -2702,7 +2703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>203</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>198</v>
       </c>
@@ -2890,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>204</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>205</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>206</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>208</v>
       </c>
@@ -3178,7 +3179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>209</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>210</v>
       </c>
@@ -3272,7 +3273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>211</v>
       </c>
@@ -3319,7 +3320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>212</v>
       </c>
@@ -3366,7 +3367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>213</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>216</v>
       </c>
@@ -3554,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>217</v>
       </c>
@@ -3601,7 +3602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>198</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>218</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>219</v>
       </c>
@@ -3745,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>220</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>198</v>
       </c>
@@ -3839,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>221</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>198</v>
       </c>
@@ -3980,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>223</v>
       </c>
@@ -4027,7 +4028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>224</v>
       </c>
@@ -4074,7 +4075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>225</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>198</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>198</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>226</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>279</v>
       </c>
@@ -4309,7 +4310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>227</v>
       </c>
@@ -4356,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>228</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>229</v>
       </c>
@@ -4450,7 +4451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>230</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>192</v>
       </c>
@@ -4544,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>231</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -4638,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -4685,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>198</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>198</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -4826,7 +4827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>233</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>198</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>198</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>198</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>234</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>235</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>236</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>237</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>238</v>
       </c>
@@ -5249,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -5299,7 +5300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>198</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>239</v>
       </c>
@@ -5393,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>240</v>
       </c>
@@ -5440,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>241</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>242</v>
       </c>
@@ -5534,7 +5535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>407</v>
       </c>
@@ -5581,7 +5582,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>243</v>
       </c>
@@ -5628,7 +5629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>244</v>
       </c>
@@ -5675,7 +5676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>245</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>198</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>246</v>
       </c>
@@ -5816,7 +5817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>247</v>
       </c>
@@ -5863,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>234</v>
       </c>
@@ -5910,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>240</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>248</v>
       </c>
@@ -6004,7 +6005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>249</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>250</v>
       </c>
@@ -6098,7 +6099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>251</v>
       </c>
@@ -6145,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>252</v>
       </c>
@@ -6192,7 +6193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>253</v>
       </c>
@@ -6239,7 +6240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>254</v>
       </c>
@@ -6286,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>255</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>256</v>
       </c>
@@ -6380,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>257</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>258</v>
       </c>
@@ -6474,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>259</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -6615,7 +6616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>260</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>261</v>
       </c>
@@ -6709,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -6756,7 +6757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>198</v>
       </c>
@@ -6803,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>262</v>
       </c>
@@ -6850,7 +6851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>263</v>
       </c>
@@ -6897,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>264</v>
       </c>
@@ -6944,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>265</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>266</v>
       </c>
@@ -7038,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>267</v>
       </c>
@@ -7085,7 +7086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>198</v>
       </c>
@@ -7132,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>268</v>
       </c>
@@ -7179,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>269</v>
       </c>
@@ -7226,7 +7227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>270</v>
       </c>
@@ -7273,7 +7274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>271</v>
       </c>
@@ -7320,7 +7321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>191</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>272</v>
       </c>
@@ -7414,7 +7415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>273</v>
       </c>
@@ -7461,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>274</v>
       </c>
@@ -7508,7 +7509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>275</v>
       </c>
@@ -7555,7 +7556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>276</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>277</v>
       </c>
@@ -7649,7 +7650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>278</v>
       </c>
@@ -7697,7 +7698,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:AG113">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:AG113">
     <sortCondition ref="E2:E113"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>